<commit_message>
Update according the review comments
</commit_message>
<xml_diff>
--- a/boston_housing/manual_calculation.xlsx
+++ b/boston_housing/manual_calculation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="14320" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="14320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="3" r:id="rId1"/>
@@ -148,7 +148,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3171,11 +3170,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="534496256"/>
-        <c:axId val="598254752"/>
+        <c:axId val="1221271344"/>
+        <c:axId val="1221276304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="534496256"/>
+        <c:axId val="1221271344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3231,12 +3230,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="598254752"/>
+        <c:crossAx val="1221276304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="598254752"/>
+        <c:axId val="1221276304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3292,7 +3291,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="534496256"/>
+        <c:crossAx val="1221271344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6379,11 +6378,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="205381664"/>
-        <c:axId val="198382896"/>
+        <c:axId val="1222092528"/>
+        <c:axId val="1222096816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="205381664"/>
+        <c:axId val="1222092528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6439,12 +6438,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198382896"/>
+        <c:crossAx val="1222096816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198382896"/>
+        <c:axId val="1222096816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6500,7 +6499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="205381664"/>
+        <c:crossAx val="1222092528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9587,11 +9586,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="198358256"/>
-        <c:axId val="200150336"/>
+        <c:axId val="1221341072"/>
+        <c:axId val="1221345360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="198358256"/>
+        <c:axId val="1221341072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9647,12 +9646,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200150336"/>
+        <c:crossAx val="1221345360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="200150336"/>
+        <c:axId val="1221345360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9708,7 +9707,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198358256"/>
+        <c:crossAx val="1221341072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11801,8 +11800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K490"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26606,7 +26605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D490"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Start project student intervention
</commit_message>
<xml_diff>
--- a/boston_housing/manual_calculation.xlsx
+++ b/boston_housing/manual_calculation.xlsx
@@ -17,6 +17,9 @@
     <sheet name="lstat_medv" sheetId="5" r:id="rId3"/>
     <sheet name="ptratio_medv" sheetId="6" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">raw_data!$C$1:$C$490</definedName>
+  </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -3170,11 +3173,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1221271344"/>
-        <c:axId val="1221276304"/>
+        <c:axId val="1310618400"/>
+        <c:axId val="1310622592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1221271344"/>
+        <c:axId val="1310618400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3230,12 +3233,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1221276304"/>
+        <c:crossAx val="1310622592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1221276304"/>
+        <c:axId val="1310622592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3291,7 +3294,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1221271344"/>
+        <c:crossAx val="1310618400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3355,7 +3358,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6378,11 +6380,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1222092528"/>
-        <c:axId val="1222096816"/>
+        <c:axId val="1310793088"/>
+        <c:axId val="1310797376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1222092528"/>
+        <c:axId val="1310793088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6438,12 +6440,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1222096816"/>
+        <c:crossAx val="1310797376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1222096816"/>
+        <c:axId val="1310797376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6499,7 +6501,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1222092528"/>
+        <c:crossAx val="1310793088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6563,7 +6565,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9586,11 +9587,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1221341072"/>
-        <c:axId val="1221345360"/>
+        <c:axId val="1272632208"/>
+        <c:axId val="1272622832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1221341072"/>
+        <c:axId val="1272632208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9646,12 +9647,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1221345360"/>
+        <c:crossAx val="1272622832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1221345360"/>
+        <c:axId val="1272622832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9707,7 +9708,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1221341072"/>
+        <c:crossAx val="1272632208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11798,10 +11799,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K490"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11884,7 +11886,7 @@
         <v>165340.27765266786</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>6.4210000000000003</v>
       </c>
@@ -11898,7 +11900,7 @@
         <v>453600</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>7.1849999999999996</v>
       </c>
@@ -11912,7 +11914,7 @@
         <v>728700</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6.9980000000000002</v>
       </c>
@@ -11926,7 +11928,7 @@
         <v>701400</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>7.1470000000000002</v>
       </c>
@@ -11940,7 +11942,7 @@
         <v>760200</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6.43</v>
       </c>
@@ -12052,7 +12054,7 @@
         <v>455700</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5.9489999999999998</v>
       </c>
@@ -12066,7 +12068,7 @@
         <v>428400</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>6.0960000000000001</v>
       </c>
@@ -12080,7 +12082,7 @@
         <v>382200</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>5.8339999999999996</v>
       </c>
@@ -12094,7 +12096,7 @@
         <v>417900</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>5.9349999999999996</v>
       </c>
@@ -12108,7 +12110,7 @@
         <v>485100</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>5.99</v>
       </c>
@@ -12122,7 +12124,7 @@
         <v>367500</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>5.4560000000000004</v>
       </c>
@@ -12136,7 +12138,7 @@
         <v>424200</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>5.7270000000000003</v>
       </c>
@@ -12150,7 +12152,7 @@
         <v>382200</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>5.57</v>
       </c>
@@ -12164,7 +12166,7 @@
         <v>285600</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5.9649999999999999</v>
       </c>
@@ -12178,7 +12180,7 @@
         <v>411600</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6.1420000000000003</v>
       </c>
@@ -12192,7 +12194,7 @@
         <v>319200</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>5.8129999999999997</v>
       </c>
@@ -12206,7 +12208,7 @@
         <v>304500</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>5.9240000000000004</v>
       </c>
@@ -12220,7 +12222,7 @@
         <v>327600</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>5.5990000000000002</v>
       </c>
@@ -12234,7 +12236,7 @@
         <v>291900</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>5.8129999999999997</v>
       </c>
@@ -12248,7 +12250,7 @@
         <v>348600</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>6.0469999999999997</v>
       </c>
@@ -12262,7 +12264,7 @@
         <v>310800</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>6.4950000000000001</v>
       </c>
@@ -12276,7 +12278,7 @@
         <v>386400</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>6.6740000000000004</v>
       </c>
@@ -12290,7 +12292,7 @@
         <v>441000</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>5.7130000000000001</v>
       </c>
@@ -12304,7 +12306,7 @@
         <v>266700</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>6.0720000000000001</v>
       </c>
@@ -12318,7 +12320,7 @@
         <v>304500</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>5.95</v>
       </c>
@@ -12332,7 +12334,7 @@
         <v>277200</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>5.7009999999999996</v>
       </c>
@@ -12346,7 +12348,7 @@
         <v>275100</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>6.0960000000000001</v>
       </c>
@@ -12360,7 +12362,7 @@
         <v>283500</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>5.9329999999999998</v>
       </c>
@@ -12374,7 +12376,7 @@
         <v>396900</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>5.8410000000000002</v>
       </c>
@@ -12388,7 +12390,7 @@
         <v>420000</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>5.85</v>
       </c>
@@ -12402,7 +12404,7 @@
         <v>441000</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>5.9660000000000002</v>
       </c>
@@ -12416,7 +12418,7 @@
         <v>518700</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>6.5949999999999998</v>
       </c>
@@ -12430,7 +12432,7 @@
         <v>646800</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>7.024</v>
       </c>
@@ -12444,7 +12446,7 @@
         <v>732900</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>6.77</v>
       </c>
@@ -12458,7 +12460,7 @@
         <v>558600</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>6.1689999999999996</v>
       </c>
@@ -12472,7 +12474,7 @@
         <v>531300</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>6.2110000000000003</v>
       </c>
@@ -12486,7 +12488,7 @@
         <v>518700</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>6.069</v>
       </c>
@@ -12500,7 +12502,7 @@
         <v>445200</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>5.6820000000000004</v>
       </c>
@@ -12514,7 +12516,7 @@
         <v>405300</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>5.7859999999999996</v>
       </c>
@@ -12528,7 +12530,7 @@
         <v>420000</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>6.03</v>
       </c>
@@ -12542,7 +12544,7 @@
         <v>348600</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>5.399</v>
       </c>
@@ -12556,7 +12558,7 @@
         <v>302400</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>5.6020000000000003</v>
       </c>
@@ -12570,7 +12572,7 @@
         <v>407400</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>5.9630000000000001</v>
       </c>
@@ -12584,7 +12586,7 @@
         <v>413700</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>6.1150000000000002</v>
       </c>
@@ -12598,7 +12600,7 @@
         <v>430500</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>6.5110000000000001</v>
       </c>
@@ -12612,7 +12614,7 @@
         <v>525000</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>5.9980000000000002</v>
       </c>
@@ -12626,7 +12628,7 @@
         <v>491400</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>5.8879999999999999</v>
       </c>
@@ -12640,7 +12642,7 @@
         <v>396900</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>7.2489999999999997</v>
       </c>
@@ -12654,7 +12656,7 @@
         <v>743400</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>6.383</v>
       </c>
@@ -12682,7 +12684,7 @@
         <v>663600</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>6.1449999999999996</v>
       </c>
@@ -12696,7 +12698,7 @@
         <v>489300</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>5.9269999999999996</v>
       </c>
@@ -12710,7 +12712,7 @@
         <v>411600</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>5.7409999999999997</v>
       </c>
@@ -12724,7 +12726,7 @@
         <v>392700</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>5.9660000000000002</v>
       </c>
@@ -12738,7 +12740,7 @@
         <v>336000</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>6.4560000000000004</v>
       </c>
@@ -12752,7 +12754,7 @@
         <v>466200</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>6.7619999999999996</v>
       </c>
@@ -12766,7 +12768,7 @@
         <v>525000</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>7.1040000000000001</v>
       </c>
@@ -12780,7 +12782,7 @@
         <v>693000</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>6.29</v>
       </c>
@@ -12794,7 +12796,7 @@
         <v>493500</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>5.7869999999999999</v>
       </c>
@@ -12808,7 +12810,7 @@
         <v>407400</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>5.8780000000000001</v>
       </c>
@@ -12822,7 +12824,7 @@
         <v>462000</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>5.5940000000000003</v>
       </c>
@@ -12836,7 +12838,7 @@
         <v>365400</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>5.8849999999999998</v>
       </c>
@@ -12850,7 +12852,7 @@
         <v>438900</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>6.4169999999999998</v>
       </c>
@@ -12864,7 +12866,7 @@
         <v>508200</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>5.9610000000000003</v>
       </c>
@@ -12878,7 +12880,7 @@
         <v>455700</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>6.0650000000000004</v>
       </c>
@@ -12892,7 +12894,7 @@
         <v>478800</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>6.2450000000000001</v>
       </c>
@@ -12906,7 +12908,7 @@
         <v>491400</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>6.2729999999999997</v>
       </c>
@@ -12920,7 +12922,7 @@
         <v>506100</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>6.2859999999999996</v>
       </c>
@@ -12934,7 +12936,7 @@
         <v>449400</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>6.2789999999999999</v>
       </c>
@@ -12948,7 +12950,7 @@
         <v>420000</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>6.14</v>
       </c>
@@ -12962,7 +12964,7 @@
         <v>436800</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>6.2320000000000002</v>
       </c>
@@ -12976,7 +12978,7 @@
         <v>445200</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>5.8739999999999997</v>
       </c>
@@ -12990,7 +12992,7 @@
         <v>426300</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>6.7270000000000003</v>
       </c>
@@ -13004,7 +13006,7 @@
         <v>588000</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>6.6189999999999998</v>
       </c>
@@ -13018,7 +13020,7 @@
         <v>501900</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>6.3019999999999996</v>
       </c>
@@ -13032,7 +13034,7 @@
         <v>520800</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>6.1669999999999998</v>
       </c>
@@ -13046,7 +13048,7 @@
         <v>480900</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>6.3890000000000002</v>
       </c>
@@ -13060,7 +13062,7 @@
         <v>501900</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>6.63</v>
       </c>
@@ -13074,7 +13076,7 @@
         <v>558600</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>6.0149999999999997</v>
       </c>
@@ -13088,7 +13090,7 @@
         <v>472500</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>6.1210000000000004</v>
       </c>
@@ -13102,7 +13104,7 @@
         <v>466200</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>7.0069999999999997</v>
       </c>
@@ -13116,7 +13118,7 @@
         <v>495600</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>7.0789999999999997</v>
       </c>
@@ -13130,7 +13132,7 @@
         <v>602700</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>6.4169999999999998</v>
       </c>
@@ -13144,7 +13146,7 @@
         <v>474600</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>6.4050000000000002</v>
       </c>
@@ -13158,7 +13160,7 @@
         <v>462000</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>6.4420000000000002</v>
       </c>
@@ -13172,7 +13174,7 @@
         <v>480900</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>6.2110000000000003</v>
       </c>
@@ -13186,7 +13188,7 @@
         <v>525000</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>6.2489999999999997</v>
       </c>
@@ -13200,7 +13202,7 @@
         <v>432600</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>6.625</v>
       </c>
@@ -13214,7 +13216,7 @@
         <v>596400</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>6.1630000000000003</v>
       </c>
@@ -13228,7 +13230,7 @@
         <v>449400</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>8.0690000000000008</v>
       </c>
@@ -13242,7 +13244,7 @@
         <v>812700</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>7.82</v>
       </c>
@@ -13256,7 +13258,7 @@
         <v>919800</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>7.4160000000000004</v>
       </c>
@@ -13270,7 +13272,7 @@
         <v>697200</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>6.7270000000000003</v>
       </c>
@@ -13284,7 +13286,7 @@
         <v>577500</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>6.7809999999999997</v>
       </c>
@@ -13298,7 +13300,7 @@
         <v>556500</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>6.4050000000000002</v>
       </c>
@@ -13312,7 +13314,7 @@
         <v>390600</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>6.1369999999999996</v>
       </c>
@@ -13326,7 +13328,7 @@
         <v>405300</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>6.1669999999999998</v>
       </c>
@@ -13340,7 +13342,7 @@
         <v>422100</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>5.851</v>
       </c>
@@ -13354,7 +13356,7 @@
         <v>409500</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>5.8360000000000003</v>
       </c>
@@ -13368,7 +13370,7 @@
         <v>409500</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>6.1269999999999998</v>
       </c>
@@ -13382,7 +13384,7 @@
         <v>428400</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>6.4740000000000002</v>
       </c>
@@ -13396,7 +13398,7 @@
         <v>415800</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>6.2290000000000001</v>
       </c>
@@ -13410,7 +13412,7 @@
         <v>407400</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>6.1950000000000003</v>
       </c>
@@ -13424,7 +13426,7 @@
         <v>455700</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>6.7149999999999999</v>
       </c>
@@ -13438,7 +13440,7 @@
         <v>478800</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>5.9130000000000003</v>
       </c>
@@ -13452,7 +13454,7 @@
         <v>394800</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>6.0919999999999996</v>
       </c>
@@ -13466,7 +13468,7 @@
         <v>392700</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>6.2539999999999996</v>
       </c>
@@ -13480,7 +13482,7 @@
         <v>388500</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>5.9279999999999999</v>
       </c>
@@ -13494,7 +13496,7 @@
         <v>384300</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>6.1760000000000002</v>
       </c>
@@ -13508,7 +13510,7 @@
         <v>445200</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>6.0209999999999999</v>
       </c>
@@ -13522,7 +13524,7 @@
         <v>403200</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>5.8719999999999999</v>
       </c>
@@ -13536,7 +13538,7 @@
         <v>428400</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>5.7309999999999999</v>
       </c>
@@ -13550,7 +13552,7 @@
         <v>405300</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>5.87</v>
       </c>
@@ -13564,7 +13566,7 @@
         <v>462000</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>6.0039999999999996</v>
       </c>
@@ -13578,7 +13580,7 @@
         <v>426300</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>5.9610000000000003</v>
       </c>
@@ -13592,7 +13594,7 @@
         <v>430500</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>5.8559999999999999</v>
       </c>
@@ -13606,7 +13608,7 @@
         <v>363300</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>5.8789999999999996</v>
       </c>
@@ -13620,7 +13622,7 @@
         <v>394800</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>5.9859999999999998</v>
       </c>
@@ -13634,7 +13636,7 @@
         <v>449400</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>5.6130000000000004</v>
       </c>
@@ -13648,7 +13650,7 @@
         <v>329700</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>5.6929999999999996</v>
       </c>
@@ -13662,7 +13664,7 @@
         <v>340200</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>6.431</v>
       </c>
@@ -13676,7 +13678,7 @@
         <v>378000</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>5.6369999999999996</v>
       </c>
@@ -13690,7 +13692,7 @@
         <v>300300</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>6.4580000000000002</v>
       </c>
@@ -13704,7 +13706,7 @@
         <v>403200</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>6.3259999999999996</v>
       </c>
@@ -13718,7 +13720,7 @@
         <v>411600</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>6.3719999999999999</v>
       </c>
@@ -13732,7 +13734,7 @@
         <v>483000</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>5.8220000000000001</v>
       </c>
@@ -13746,7 +13748,7 @@
         <v>386400</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>5.7569999999999997</v>
       </c>
@@ -13760,7 +13762,7 @@
         <v>327600</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>6.335</v>
       </c>
@@ -13774,7 +13776,7 @@
         <v>380100</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>5.9420000000000002</v>
       </c>
@@ -13788,7 +13790,7 @@
         <v>365400</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>6.4539999999999997</v>
       </c>
@@ -13802,7 +13804,7 @@
         <v>359100</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>5.8570000000000002</v>
       </c>
@@ -13816,7 +13818,7 @@
         <v>279300</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>6.1509999999999998</v>
       </c>
@@ -13830,7 +13832,7 @@
         <v>373800</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>6.1740000000000004</v>
       </c>
@@ -13844,7 +13846,7 @@
         <v>294000</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>5.0190000000000001</v>
       </c>
@@ -14222,7 +14224,7 @@
         <v>401100</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>5.5720000000000001</v>
       </c>
@@ -14236,7 +14238,7 @@
         <v>485100</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>6.4160000000000004</v>
       </c>
@@ -14250,7 +14252,7 @@
         <v>495600</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>5.859</v>
       </c>
@@ -14264,7 +14266,7 @@
         <v>474600</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>6.5460000000000003</v>
       </c>
@@ -14278,7 +14280,7 @@
         <v>617400</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>6.02</v>
       </c>
@@ -14292,7 +14294,7 @@
         <v>487200</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>6.3150000000000004</v>
       </c>
@@ -14306,7 +14308,7 @@
         <v>516600</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>6.86</v>
       </c>
@@ -14320,7 +14322,7 @@
         <v>627900</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>6.98</v>
       </c>
@@ -14334,7 +14336,7 @@
         <v>781200</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>7.7649999999999997</v>
       </c>
@@ -14348,7 +14350,7 @@
         <v>835800</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>6.1440000000000001</v>
       </c>
@@ -14362,7 +14364,7 @@
         <v>760200</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>7.1550000000000002</v>
       </c>
@@ -14376,7 +14378,7 @@
         <v>795900</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>6.5629999999999997</v>
       </c>
@@ -14390,7 +14392,7 @@
         <v>682500</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>5.6040000000000001</v>
       </c>
@@ -14404,7 +14406,7 @@
         <v>554400</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>6.1529999999999996</v>
       </c>
@@ -14502,7 +14504,7 @@
         <v>764400</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>6.8</v>
       </c>
@@ -14516,7 +14518,7 @@
         <v>653100</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>6.6040000000000001</v>
       </c>
@@ -14530,7 +14532,7 @@
         <v>611100</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>7.2869999999999999</v>
       </c>
@@ -14544,7 +14546,7 @@
         <v>699300</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>7.1070000000000002</v>
       </c>
@@ -14558,7 +14560,7 @@
         <v>636300</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>7.274</v>
       </c>
@@ -14572,7 +14574,7 @@
         <v>726600</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>6.9749999999999996</v>
       </c>
@@ -14586,7 +14588,7 @@
         <v>732900</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>7.1349999999999998</v>
       </c>
@@ -14642,7 +14644,7 @@
         <v>1018500</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>5.891</v>
       </c>
@@ -14656,7 +14658,7 @@
         <v>474600</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>6.3259999999999996</v>
       </c>
@@ -14670,7 +14672,7 @@
         <v>512400</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>5.7830000000000004</v>
       </c>
@@ -14684,7 +14686,7 @@
         <v>472500</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>6.0640000000000001</v>
       </c>
@@ -14698,7 +14700,7 @@
         <v>512400</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>5.3440000000000003</v>
       </c>
@@ -14712,7 +14714,7 @@
         <v>420000</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>5.96</v>
       </c>
@@ -14726,7 +14728,7 @@
         <v>455700</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>5.4039999999999999</v>
       </c>
@@ -14740,7 +14742,7 @@
         <v>405300</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>5.8070000000000004</v>
       </c>
@@ -14754,7 +14756,7 @@
         <v>470400</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>6.375</v>
       </c>
@@ -14768,7 +14770,7 @@
         <v>590100</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>5.4119999999999999</v>
       </c>
@@ -14782,7 +14784,7 @@
         <v>497700</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>6.1820000000000004</v>
       </c>
@@ -14796,7 +14798,7 @@
         <v>525000</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>5.8879999999999999</v>
       </c>
@@ -14810,7 +14812,7 @@
         <v>489300</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>6.6420000000000003</v>
       </c>
@@ -14824,7 +14826,7 @@
         <v>602700</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>5.9509999999999996</v>
       </c>
@@ -14838,7 +14840,7 @@
         <v>451500</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>6.3730000000000002</v>
       </c>
@@ -14852,7 +14854,7 @@
         <v>483000</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>6.9509999999999996</v>
       </c>
@@ -14866,7 +14868,7 @@
         <v>560700</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>6.1639999999999997</v>
       </c>
@@ -14880,7 +14882,7 @@
         <v>455700</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>6.8789999999999996</v>
       </c>
@@ -14894,7 +14896,7 @@
         <v>577500</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>6.6180000000000003</v>
       </c>
@@ -14908,7 +14910,7 @@
         <v>632100</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>8.266</v>
       </c>
@@ -14922,7 +14924,7 @@
         <v>940800</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>8.0399999999999991</v>
       </c>
@@ -14936,7 +14938,7 @@
         <v>789600</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>7.1630000000000003</v>
       </c>
@@ -14950,7 +14952,7 @@
         <v>663600</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>7.6859999999999999</v>
       </c>
@@ -14964,7 +14966,7 @@
         <v>980700</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>6.5519999999999996</v>
       </c>
@@ -14978,7 +14980,7 @@
         <v>661500</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>5.9809999999999999</v>
       </c>
@@ -14992,7 +14994,7 @@
         <v>510300</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>7.4119999999999999</v>
       </c>
@@ -15006,7 +15008,7 @@
         <v>665700</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>8.3369999999999997</v>
       </c>
@@ -15020,7 +15022,7 @@
         <v>875700</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>8.2469999999999999</v>
       </c>
@@ -15034,7 +15036,7 @@
         <v>1014300</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>6.726</v>
       </c>
@@ -15048,7 +15050,7 @@
         <v>609000</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>6.0860000000000003</v>
       </c>
@@ -15062,7 +15064,7 @@
         <v>504000</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>6.6310000000000002</v>
       </c>
@@ -15076,7 +15078,7 @@
         <v>527100</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>7.3579999999999997</v>
       </c>
@@ -15090,7 +15092,7 @@
         <v>661500</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>6.4809999999999999</v>
       </c>
@@ -15104,7 +15106,7 @@
         <v>497700</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>6.6059999999999999</v>
       </c>
@@ -15118,7 +15120,7 @@
         <v>489300</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>6.8970000000000002</v>
       </c>
@@ -15132,7 +15134,7 @@
         <v>462000</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>6.0949999999999998</v>
       </c>
@@ -15146,7 +15148,7 @@
         <v>422100</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>6.3579999999999997</v>
       </c>
@@ -15160,7 +15162,7 @@
         <v>466200</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>6.3929999999999998</v>
       </c>
@@ -15174,7 +15176,7 @@
         <v>497700</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>5.593</v>
       </c>
@@ -15188,7 +15190,7 @@
         <v>369600</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>5.6050000000000004</v>
       </c>
@@ -15202,7 +15204,7 @@
         <v>388500</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>6.1079999999999997</v>
       </c>
@@ -15216,7 +15218,7 @@
         <v>510300</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>6.226</v>
       </c>
@@ -15230,7 +15232,7 @@
         <v>430500</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>6.4329999999999998</v>
       </c>
@@ -15244,7 +15246,7 @@
         <v>514500</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>6.718</v>
       </c>
@@ -15258,7 +15260,7 @@
         <v>550200</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>6.4870000000000001</v>
       </c>
@@ -15272,7 +15274,7 @@
         <v>512400</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>6.4379999999999997</v>
       </c>
@@ -15286,7 +15288,7 @@
         <v>520800</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>6.9569999999999999</v>
       </c>
@@ -15300,7 +15302,7 @@
         <v>621600</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>8.2590000000000003</v>
       </c>
@@ -15314,7 +15316,7 @@
         <v>898800</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>6.1079999999999997</v>
       </c>
@@ -15328,7 +15330,7 @@
         <v>459900</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>5.8760000000000003</v>
       </c>
@@ -15342,7 +15344,7 @@
         <v>438900</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>7.4539999999999997</v>
       </c>
@@ -15356,7 +15358,7 @@
         <v>924000</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>7.3330000000000002</v>
       </c>
@@ -15370,7 +15372,7 @@
         <v>756000</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>6.8419999999999996</v>
       </c>
@@ -15384,7 +15386,7 @@
         <v>632100</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>7.2030000000000003</v>
       </c>
@@ -15398,7 +15400,7 @@
         <v>709800</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>7.52</v>
       </c>
@@ -15412,7 +15414,7 @@
         <v>905100</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>8.3979999999999997</v>
       </c>
@@ -15426,7 +15428,7 @@
         <v>1024800</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>7.327</v>
       </c>
@@ -15440,7 +15442,7 @@
         <v>651000</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>7.2060000000000004</v>
       </c>
@@ -15454,7 +15456,7 @@
         <v>766500</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>5.56</v>
       </c>
@@ -15468,7 +15470,7 @@
         <v>478800</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>7.0140000000000002</v>
       </c>
@@ -15482,7 +15484,7 @@
         <v>644700</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>7.47</v>
       </c>
@@ -15496,7 +15498,7 @@
         <v>913500</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>5.92</v>
       </c>
@@ -15510,7 +15512,7 @@
         <v>434700</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>5.8559999999999999</v>
       </c>
@@ -15524,7 +15526,7 @@
         <v>443100</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>6.24</v>
       </c>
@@ -15538,7 +15540,7 @@
         <v>529200</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>6.5380000000000003</v>
       </c>
@@ -15552,7 +15554,7 @@
         <v>512400</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>7.6909999999999998</v>
       </c>
@@ -15566,7 +15568,7 @@
         <v>739200</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>6.758</v>
       </c>
@@ -15580,7 +15582,7 @@
         <v>680400</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>6.8540000000000001</v>
       </c>
@@ -15594,7 +15596,7 @@
         <v>672000</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>7.2670000000000003</v>
       </c>
@@ -15608,7 +15610,7 @@
         <v>697200</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>6.8259999999999996</v>
       </c>
@@ -15622,7 +15624,7 @@
         <v>695100</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>6.4820000000000002</v>
       </c>
@@ -15720,7 +15722,7 @@
         <v>462000</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>6.23</v>
       </c>
@@ -15734,7 +15736,7 @@
         <v>422100</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>6.2089999999999996</v>
       </c>
@@ -15748,7 +15750,7 @@
         <v>487200</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>6.3150000000000004</v>
       </c>
@@ -15762,7 +15764,7 @@
         <v>468300</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>6.5650000000000004</v>
       </c>
@@ -15776,7 +15778,7 @@
         <v>520800</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>6.8609999999999998</v>
       </c>
@@ -15790,7 +15792,7 @@
         <v>598500</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>7.1479999999999997</v>
       </c>
@@ -15804,7 +15806,7 @@
         <v>783300</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>6.63</v>
       </c>
@@ -15818,7 +15820,7 @@
         <v>585900</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>6.1269999999999998</v>
       </c>
@@ -15832,7 +15834,7 @@
         <v>501900</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>6.0090000000000003</v>
       </c>
@@ -15846,7 +15848,7 @@
         <v>455700</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>6.6779999999999999</v>
       </c>
@@ -15860,7 +15862,7 @@
         <v>600600</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>6.5490000000000004</v>
       </c>
@@ -15874,7 +15876,7 @@
         <v>569100</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>5.79</v>
       </c>
@@ -15930,7 +15932,7 @@
         <v>520800</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>6.59</v>
       </c>
@@ -15944,7 +15946,7 @@
         <v>462000</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>6.4950000000000001</v>
       </c>
@@ -15958,7 +15960,7 @@
         <v>554400</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>6.9820000000000002</v>
       </c>
@@ -15972,7 +15974,7 @@
         <v>695100</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>7.2359999999999998</v>
       </c>
@@ -15986,7 +15988,7 @@
         <v>758100</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>6.6159999999999997</v>
       </c>
@@ -16000,7 +16002,7 @@
         <v>596400</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>7.42</v>
       </c>
@@ -16014,7 +16016,7 @@
         <v>701400</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>6.8490000000000002</v>
       </c>
@@ -16028,7 +16030,7 @@
         <v>592200</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>6.6349999999999998</v>
       </c>
@@ -16042,7 +16044,7 @@
         <v>478800</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>5.9720000000000004</v>
       </c>
@@ -16056,7 +16058,7 @@
         <v>426300</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>4.9729999999999999</v>
       </c>
@@ -16070,7 +16072,7 @@
         <v>338100</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>6.1219999999999999</v>
       </c>
@@ -16084,7 +16086,7 @@
         <v>464100</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>6.0229999999999997</v>
       </c>
@@ -16098,7 +16100,7 @@
         <v>407400</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>6.266</v>
       </c>
@@ -16112,7 +16114,7 @@
         <v>453600</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>6.5670000000000002</v>
       </c>
@@ -16126,7 +16128,7 @@
         <v>499800</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>5.7050000000000001</v>
       </c>
@@ -16140,7 +16142,7 @@
         <v>340200</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>5.9139999999999997</v>
       </c>
@@ -16154,7 +16156,7 @@
         <v>373800</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>5.782</v>
       </c>
@@ -16168,7 +16170,7 @@
         <v>415800</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>6.3819999999999997</v>
       </c>
@@ -16182,7 +16184,7 @@
         <v>485100</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>6.1130000000000004</v>
       </c>
@@ -16196,7 +16198,7 @@
         <v>441000</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>6.4260000000000002</v>
       </c>
@@ -16210,7 +16212,7 @@
         <v>499800</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>6.3760000000000003</v>
       </c>
@@ -16224,7 +16226,7 @@
         <v>485100</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>6.0410000000000004</v>
       </c>
@@ -16238,7 +16240,7 @@
         <v>428400</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>5.7080000000000002</v>
       </c>
@@ -16252,7 +16254,7 @@
         <v>388500</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>6.415</v>
       </c>
@@ -16266,7 +16268,7 @@
         <v>525000</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>6.431</v>
       </c>
@@ -16280,7 +16282,7 @@
         <v>516600</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>6.3120000000000003</v>
       </c>
@@ -16294,7 +16296,7 @@
         <v>483000</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>6.0830000000000002</v>
       </c>
@@ -16308,7 +16310,7 @@
         <v>466200</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>5.8680000000000003</v>
       </c>
@@ -16322,7 +16324,7 @@
         <v>405300</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>6.3330000000000002</v>
       </c>
@@ -16336,7 +16338,7 @@
         <v>474600</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>6.1440000000000001</v>
       </c>
@@ -16350,7 +16352,7 @@
         <v>415800</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>5.7060000000000004</v>
       </c>
@@ -16364,7 +16366,7 @@
         <v>359100</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>6.0309999999999997</v>
       </c>
@@ -16378,7 +16380,7 @@
         <v>407400</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>6.3159999999999998</v>
       </c>
@@ -16392,7 +16394,7 @@
         <v>466200</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>6.31</v>
       </c>
@@ -16406,7 +16408,7 @@
         <v>434700</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>6.0369999999999999</v>
       </c>
@@ -16420,7 +16422,7 @@
         <v>443100</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>5.8689999999999998</v>
       </c>
@@ -16434,7 +16436,7 @@
         <v>409500</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>5.8949999999999996</v>
       </c>
@@ -16448,7 +16450,7 @@
         <v>388500</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>6.0590000000000002</v>
       </c>
@@ -16462,7 +16464,7 @@
         <v>432600</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>5.9850000000000003</v>
       </c>
@@ -16476,7 +16478,7 @@
         <v>399000</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>5.968</v>
       </c>
@@ -16504,7 +16506,7 @@
         <v>686700</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>6.54</v>
       </c>
@@ -16518,7 +16520,7 @@
         <v>346500</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>6.6959999999999997</v>
       </c>
@@ -16532,7 +16534,7 @@
         <v>501900</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>6.8739999999999997</v>
       </c>
@@ -16546,7 +16548,7 @@
         <v>655200</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>6.0140000000000002</v>
       </c>
@@ -16560,7 +16562,7 @@
         <v>367500</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>5.8979999999999997</v>
       </c>
@@ -16574,7 +16576,7 @@
         <v>361200</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>6.516</v>
       </c>
@@ -16588,7 +16590,7 @@
         <v>485100</v>
       </c>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>6.6349999999999998</v>
       </c>
@@ -16602,7 +16604,7 @@
         <v>514500</v>
       </c>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>6.9390000000000001</v>
       </c>
@@ -16616,7 +16618,7 @@
         <v>558600</v>
       </c>
     </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>6.49</v>
       </c>
@@ -16630,7 +16632,7 @@
         <v>480900</v>
       </c>
     </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>6.5789999999999997</v>
       </c>
@@ -16644,7 +16646,7 @@
         <v>506100</v>
       </c>
     </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>5.8840000000000003</v>
       </c>
@@ -16658,7 +16660,7 @@
         <v>390600</v>
       </c>
     </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>6.7279999999999998</v>
       </c>
@@ -16672,7 +16674,7 @@
         <v>632100</v>
       </c>
     </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>5.6630000000000003</v>
       </c>
@@ -16686,7 +16688,7 @@
         <v>382200</v>
       </c>
     </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>5.9359999999999999</v>
       </c>
@@ -16700,7 +16702,7 @@
         <v>432600</v>
       </c>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>6.2119999999999997</v>
       </c>
@@ -16714,7 +16716,7 @@
         <v>373800</v>
       </c>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>6.3949999999999996</v>
       </c>
@@ -16728,7 +16730,7 @@
         <v>455700</v>
       </c>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>6.1269999999999998</v>
       </c>
@@ -16742,7 +16744,7 @@
         <v>476700</v>
       </c>
     </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A350">
         <v>6.1120000000000001</v>
       </c>
@@ -16756,7 +16758,7 @@
         <v>474600</v>
       </c>
     </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A351">
         <v>6.3979999999999997</v>
       </c>
@@ -16770,7 +16772,7 @@
         <v>525000</v>
       </c>
     </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A352">
         <v>6.2510000000000003</v>
       </c>
@@ -16784,7 +16786,7 @@
         <v>417900</v>
       </c>
     </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A353">
         <v>5.3620000000000001</v>
       </c>
@@ -16798,7 +16800,7 @@
         <v>436800</v>
       </c>
     </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A354">
         <v>5.8029999999999999</v>
       </c>
@@ -16812,7 +16814,7 @@
         <v>352800</v>
       </c>
     </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>3.5609999999999999</v>
       </c>
@@ -16826,7 +16828,7 @@
         <v>577500</v>
       </c>
     </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A356">
         <v>4.9630000000000001</v>
       </c>
@@ -16840,7 +16842,7 @@
         <v>459900</v>
       </c>
     </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A357">
         <v>3.863</v>
       </c>
@@ -16854,7 +16856,7 @@
         <v>485100</v>
       </c>
     </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A358">
         <v>4.9059999999999997</v>
       </c>
@@ -16868,7 +16870,7 @@
         <v>289800</v>
       </c>
     </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A359">
         <v>4.1379999999999999</v>
       </c>
@@ -16882,7 +16884,7 @@
         <v>289800</v>
       </c>
     </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A360">
         <v>7.3129999999999997</v>
       </c>
@@ -16896,7 +16898,7 @@
         <v>315000</v>
       </c>
     </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A361">
         <v>6.649</v>
       </c>
@@ -16910,7 +16912,7 @@
         <v>291900</v>
       </c>
     </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A362">
         <v>6.7939999999999996</v>
       </c>
@@ -16924,7 +16926,7 @@
         <v>279300</v>
       </c>
     </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A363">
         <v>6.38</v>
       </c>
@@ -16938,7 +16940,7 @@
         <v>275100</v>
       </c>
     </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A364">
         <v>6.2229999999999999</v>
       </c>
@@ -16952,7 +16954,7 @@
         <v>214200</v>
       </c>
     </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A365">
         <v>6.968</v>
       </c>
@@ -16966,7 +16968,7 @@
         <v>218400</v>
       </c>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A366">
         <v>6.5449999999999999</v>
       </c>
@@ -16980,7 +16982,7 @@
         <v>228900</v>
       </c>
     </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A367">
         <v>5.5359999999999996</v>
       </c>
@@ -16994,7 +16996,7 @@
         <v>237300</v>
       </c>
     </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A368">
         <v>5.52</v>
       </c>
@@ -17008,7 +17010,7 @@
         <v>258300</v>
       </c>
     </row>
-    <row r="369" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>4.3680000000000003</v>
       </c>
@@ -17022,7 +17024,7 @@
         <v>184800</v>
       </c>
     </row>
-    <row r="370" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>5.2770000000000001</v>
       </c>
@@ -17036,7 +17038,7 @@
         <v>151200</v>
       </c>
     </row>
-    <row r="371" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A371">
         <v>4.6520000000000001</v>
       </c>
@@ -17050,7 +17052,7 @@
         <v>220500</v>
       </c>
     </row>
-    <row r="372" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A372">
         <v>5</v>
       </c>
@@ -17064,7 +17066,7 @@
         <v>155400</v>
       </c>
     </row>
-    <row r="373" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A373">
         <v>4.88</v>
       </c>
@@ -17078,7 +17080,7 @@
         <v>214200</v>
       </c>
     </row>
-    <row r="374" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A374">
         <v>5.39</v>
       </c>
@@ -17092,7 +17094,7 @@
         <v>241500</v>
       </c>
     </row>
-    <row r="375" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A375">
         <v>5.7130000000000001</v>
       </c>
@@ -17106,7 +17108,7 @@
         <v>317100</v>
       </c>
     </row>
-    <row r="376" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A376">
         <v>6.0510000000000002</v>
       </c>
@@ -17120,7 +17122,7 @@
         <v>487200</v>
       </c>
     </row>
-    <row r="377" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A377">
         <v>5.0359999999999996</v>
       </c>
@@ -17134,7 +17136,7 @@
         <v>203700</v>
       </c>
     </row>
-    <row r="378" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A378">
         <v>6.1929999999999996</v>
       </c>
@@ -17148,7 +17150,7 @@
         <v>289800</v>
       </c>
     </row>
-    <row r="379" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>5.8869999999999996</v>
       </c>
@@ -17162,7 +17164,7 @@
         <v>266700</v>
       </c>
     </row>
-    <row r="380" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A380">
         <v>6.4710000000000001</v>
       </c>
@@ -17176,7 +17178,7 @@
         <v>275100</v>
       </c>
     </row>
-    <row r="381" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A381">
         <v>6.4050000000000002</v>
       </c>
@@ -17190,7 +17192,7 @@
         <v>262500</v>
       </c>
     </row>
-    <row r="382" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>5.7469999999999999</v>
       </c>
@@ -17204,7 +17206,7 @@
         <v>178500</v>
       </c>
     </row>
-    <row r="383" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A383">
         <v>5.4530000000000003</v>
       </c>
@@ -17218,7 +17220,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="384" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A384">
         <v>5.8520000000000003</v>
       </c>
@@ -17232,7 +17234,7 @@
         <v>132300</v>
       </c>
     </row>
-    <row r="385" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>5.9870000000000001</v>
       </c>
@@ -17246,7 +17248,7 @@
         <v>117600</v>
       </c>
     </row>
-    <row r="386" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A386">
         <v>6.343</v>
       </c>
@@ -17260,7 +17262,7 @@
         <v>151200</v>
       </c>
     </row>
-    <row r="387" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A387">
         <v>6.4039999999999999</v>
       </c>
@@ -17274,7 +17276,7 @@
         <v>254100</v>
       </c>
     </row>
-    <row r="388" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A388">
         <v>5.3490000000000002</v>
       </c>
@@ -17288,7 +17290,7 @@
         <v>174300</v>
       </c>
     </row>
-    <row r="389" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A389">
         <v>5.5309999999999997</v>
       </c>
@@ -17302,7 +17304,7 @@
         <v>178500</v>
       </c>
     </row>
-    <row r="390" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A390">
         <v>5.6829999999999998</v>
       </c>
@@ -17316,7 +17318,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="391" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A391">
         <v>4.1379999999999999</v>
       </c>
@@ -17330,7 +17332,7 @@
         <v>249900</v>
       </c>
     </row>
-    <row r="392" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A392">
         <v>5.6079999999999997</v>
       </c>
@@ -17344,7 +17346,7 @@
         <v>585900</v>
       </c>
     </row>
-    <row r="393" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A393">
         <v>5.617</v>
       </c>
@@ -17358,7 +17360,7 @@
         <v>361200</v>
       </c>
     </row>
-    <row r="394" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A394">
         <v>6.8520000000000003</v>
       </c>
@@ -17372,7 +17374,7 @@
         <v>577500</v>
       </c>
     </row>
-    <row r="395" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A395">
         <v>5.7569999999999997</v>
       </c>
@@ -17386,7 +17388,7 @@
         <v>315000</v>
       </c>
     </row>
-    <row r="396" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A396">
         <v>6.657</v>
       </c>
@@ -17400,7 +17402,7 @@
         <v>361200</v>
       </c>
     </row>
-    <row r="397" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A397">
         <v>4.6280000000000001</v>
       </c>
@@ -17414,7 +17416,7 @@
         <v>375900</v>
       </c>
     </row>
-    <row r="398" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A398">
         <v>5.1550000000000002</v>
       </c>
@@ -17428,7 +17430,7 @@
         <v>342300</v>
       </c>
     </row>
-    <row r="399" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A399">
         <v>4.5190000000000001</v>
       </c>
@@ -17442,7 +17444,7 @@
         <v>147000</v>
       </c>
     </row>
-    <row r="400" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A400">
         <v>6.4340000000000002</v>
       </c>
@@ -17456,7 +17458,7 @@
         <v>151200</v>
       </c>
     </row>
-    <row r="401" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A401">
         <v>6.782</v>
       </c>
@@ -17470,7 +17472,7 @@
         <v>157500</v>
       </c>
     </row>
-    <row r="402" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A402">
         <v>5.3040000000000003</v>
       </c>
@@ -17484,7 +17486,7 @@
         <v>218400</v>
       </c>
     </row>
-    <row r="403" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A403">
         <v>5.9569999999999999</v>
       </c>
@@ -17498,7 +17500,7 @@
         <v>184800</v>
       </c>
     </row>
-    <row r="404" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A404">
         <v>6.8239999999999998</v>
       </c>
@@ -17512,7 +17514,7 @@
         <v>176400</v>
       </c>
     </row>
-    <row r="405" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A405">
         <v>6.4109999999999996</v>
       </c>
@@ -17526,7 +17528,7 @@
         <v>350700</v>
       </c>
     </row>
-    <row r="406" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A406">
         <v>6.0060000000000002</v>
       </c>
@@ -17540,7 +17542,7 @@
         <v>298200</v>
       </c>
     </row>
-    <row r="407" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A407">
         <v>5.6479999999999997</v>
       </c>
@@ -17554,7 +17556,7 @@
         <v>436800</v>
       </c>
     </row>
-    <row r="408" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A408">
         <v>6.1029999999999998</v>
       </c>
@@ -17568,7 +17570,7 @@
         <v>281400</v>
       </c>
     </row>
-    <row r="409" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A409">
         <v>5.5650000000000004</v>
       </c>
@@ -17582,7 +17584,7 @@
         <v>245700</v>
       </c>
     </row>
-    <row r="410" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A410">
         <v>5.8959999999999999</v>
       </c>
@@ -17596,7 +17598,7 @@
         <v>174300</v>
       </c>
     </row>
-    <row r="411" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A411">
         <v>5.8369999999999997</v>
       </c>
@@ -17610,7 +17612,7 @@
         <v>214200</v>
       </c>
     </row>
-    <row r="412" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A412">
         <v>6.202</v>
       </c>
@@ -17624,7 +17626,7 @@
         <v>228900</v>
       </c>
     </row>
-    <row r="413" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A413">
         <v>6.1929999999999996</v>
       </c>
@@ -17638,7 +17640,7 @@
         <v>231000</v>
       </c>
     </row>
-    <row r="414" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A414">
         <v>6.38</v>
       </c>
@@ -17652,7 +17654,7 @@
         <v>199500</v>
       </c>
     </row>
-    <row r="415" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A415">
         <v>6.3479999999999999</v>
       </c>
@@ -17666,7 +17668,7 @@
         <v>304500</v>
       </c>
     </row>
-    <row r="416" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A416">
         <v>6.8330000000000002</v>
       </c>
@@ -17680,7 +17682,7 @@
         <v>296100</v>
       </c>
     </row>
-    <row r="417" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A417">
         <v>6.4249999999999998</v>
       </c>
@@ -17694,7 +17696,7 @@
         <v>338100</v>
       </c>
     </row>
-    <row r="418" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A418">
         <v>6.4359999999999999</v>
       </c>
@@ -17708,7 +17710,7 @@
         <v>300300</v>
       </c>
     </row>
-    <row r="419" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A419">
         <v>6.2080000000000002</v>
       </c>
@@ -17722,7 +17724,7 @@
         <v>245700</v>
       </c>
     </row>
-    <row r="420" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A420">
         <v>6.6289999999999996</v>
       </c>
@@ -17736,7 +17738,7 @@
         <v>281400</v>
       </c>
     </row>
-    <row r="421" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A421">
         <v>6.4610000000000003</v>
       </c>
@@ -17750,7 +17752,7 @@
         <v>201600</v>
       </c>
     </row>
-    <row r="422" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A422">
         <v>6.1520000000000001</v>
       </c>
@@ -17764,7 +17766,7 @@
         <v>182700</v>
       </c>
     </row>
-    <row r="423" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A423">
         <v>5.9349999999999996</v>
       </c>
@@ -17778,7 +17780,7 @@
         <v>176400</v>
       </c>
     </row>
-    <row r="424" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A424">
         <v>5.6269999999999998</v>
       </c>
@@ -17792,7 +17794,7 @@
         <v>268800</v>
       </c>
     </row>
-    <row r="425" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A425">
         <v>5.8179999999999996</v>
       </c>
@@ -17806,7 +17808,7 @@
         <v>220500</v>
       </c>
     </row>
-    <row r="426" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A426">
         <v>6.4059999999999997</v>
       </c>
@@ -17820,7 +17822,7 @@
         <v>359100</v>
       </c>
     </row>
-    <row r="427" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A427">
         <v>6.2190000000000003</v>
       </c>
@@ -17834,7 +17836,7 @@
         <v>386400</v>
       </c>
     </row>
-    <row r="428" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A428">
         <v>6.4850000000000003</v>
       </c>
@@ -17848,7 +17850,7 @@
         <v>323400</v>
       </c>
     </row>
-    <row r="429" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A429">
         <v>5.8540000000000001</v>
       </c>
@@ -17862,7 +17864,7 @@
         <v>226800</v>
       </c>
     </row>
-    <row r="430" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A430">
         <v>6.4589999999999996</v>
       </c>
@@ -17876,7 +17878,7 @@
         <v>247800</v>
       </c>
     </row>
-    <row r="431" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A431">
         <v>6.3410000000000002</v>
       </c>
@@ -17890,7 +17892,7 @@
         <v>312900</v>
       </c>
     </row>
-    <row r="432" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A432">
         <v>6.2510000000000003</v>
       </c>
@@ -17904,7 +17906,7 @@
         <v>264600</v>
       </c>
     </row>
-    <row r="433" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A433">
         <v>6.1849999999999996</v>
       </c>
@@ -17918,7 +17920,7 @@
         <v>296100</v>
       </c>
     </row>
-    <row r="434" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A434">
         <v>6.4169999999999998</v>
       </c>
@@ -17932,7 +17934,7 @@
         <v>273000</v>
       </c>
     </row>
-    <row r="435" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A435">
         <v>6.7489999999999997</v>
       </c>
@@ -17946,7 +17948,7 @@
         <v>281400</v>
       </c>
     </row>
-    <row r="436" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A436">
         <v>6.6550000000000002</v>
       </c>
@@ -17960,7 +17962,7 @@
         <v>319200</v>
       </c>
     </row>
-    <row r="437" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A437">
         <v>6.2969999999999997</v>
       </c>
@@ -17974,7 +17976,7 @@
         <v>338100</v>
       </c>
     </row>
-    <row r="438" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A438">
         <v>7.3929999999999998</v>
       </c>
@@ -17988,7 +17990,7 @@
         <v>373800</v>
       </c>
     </row>
-    <row r="439" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A439">
         <v>6.7279999999999998</v>
       </c>
@@ -18002,7 +18004,7 @@
         <v>312900</v>
       </c>
     </row>
-    <row r="440" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A440">
         <v>6.5250000000000004</v>
       </c>
@@ -18016,7 +18018,7 @@
         <v>296100</v>
       </c>
     </row>
-    <row r="441" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A441">
         <v>5.976</v>
       </c>
@@ -18030,7 +18032,7 @@
         <v>266700</v>
       </c>
     </row>
-    <row r="442" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A442">
         <v>5.9359999999999999</v>
       </c>
@@ -18044,7 +18046,7 @@
         <v>283500</v>
       </c>
     </row>
-    <row r="443" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A443">
         <v>6.3010000000000002</v>
       </c>
@@ -18058,7 +18060,7 @@
         <v>312900</v>
       </c>
     </row>
-    <row r="444" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A444">
         <v>6.0810000000000004</v>
       </c>
@@ -18072,7 +18074,7 @@
         <v>420000</v>
       </c>
     </row>
-    <row r="445" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A445">
         <v>6.7009999999999996</v>
       </c>
@@ -18086,7 +18088,7 @@
         <v>344400</v>
       </c>
     </row>
-    <row r="446" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A446">
         <v>6.3760000000000003</v>
       </c>
@@ -18100,7 +18102,7 @@
         <v>371700</v>
       </c>
     </row>
-    <row r="447" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A447">
         <v>6.3170000000000002</v>
       </c>
@@ -18114,7 +18116,7 @@
         <v>409500</v>
       </c>
     </row>
-    <row r="448" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A448">
         <v>6.5129999999999999</v>
       </c>
@@ -18128,7 +18130,7 @@
         <v>424200</v>
       </c>
     </row>
-    <row r="449" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A449">
         <v>6.2089999999999996</v>
       </c>
@@ -18142,7 +18144,7 @@
         <v>449400</v>
       </c>
     </row>
-    <row r="450" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A450">
         <v>5.7590000000000003</v>
       </c>
@@ -18156,7 +18158,7 @@
         <v>417900</v>
       </c>
     </row>
-    <row r="451" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A451">
         <v>5.952</v>
       </c>
@@ -18170,7 +18172,7 @@
         <v>399000</v>
       </c>
     </row>
-    <row r="452" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A452">
         <v>6.0030000000000001</v>
       </c>
@@ -18184,7 +18186,7 @@
         <v>401100</v>
       </c>
     </row>
-    <row r="453" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A453">
         <v>5.9260000000000002</v>
       </c>
@@ -18198,7 +18200,7 @@
         <v>401100</v>
       </c>
     </row>
-    <row r="454" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A454">
         <v>5.7130000000000001</v>
       </c>
@@ -18212,7 +18214,7 @@
         <v>422100</v>
       </c>
     </row>
-    <row r="455" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A455">
         <v>6.1669999999999998</v>
       </c>
@@ -18226,7 +18228,7 @@
         <v>417900</v>
       </c>
     </row>
-    <row r="456" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A456">
         <v>6.2290000000000001</v>
       </c>
@@ -18240,7 +18242,7 @@
         <v>411600</v>
       </c>
     </row>
-    <row r="457" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A457">
         <v>6.4370000000000003</v>
       </c>
@@ -18254,7 +18256,7 @@
         <v>487200</v>
       </c>
     </row>
-    <row r="458" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A458">
         <v>6.98</v>
       </c>
@@ -18268,7 +18270,7 @@
         <v>625800</v>
       </c>
     </row>
-    <row r="459" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A459">
         <v>5.4269999999999996</v>
       </c>
@@ -18282,7 +18284,7 @@
         <v>289800</v>
       </c>
     </row>
-    <row r="460" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A460">
         <v>6.1619999999999999</v>
       </c>
@@ -18296,7 +18298,7 @@
         <v>279300</v>
       </c>
     </row>
-    <row r="461" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A461">
         <v>6.484</v>
       </c>
@@ -18310,7 +18312,7 @@
         <v>350700</v>
       </c>
     </row>
-    <row r="462" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A462">
         <v>5.3040000000000003</v>
       </c>
@@ -18324,7 +18326,7 @@
         <v>252000</v>
       </c>
     </row>
-    <row r="463" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A463">
         <v>6.1849999999999996</v>
       </c>
@@ -18338,7 +18340,7 @@
         <v>306600</v>
       </c>
     </row>
-    <row r="464" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A464">
         <v>6.2290000000000001</v>
       </c>
@@ -18352,7 +18354,7 @@
         <v>449400</v>
       </c>
     </row>
-    <row r="465" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A465">
         <v>6.242</v>
       </c>
@@ -18366,7 +18368,7 @@
         <v>483000</v>
       </c>
     </row>
-    <row r="466" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A466">
         <v>6.75</v>
       </c>
@@ -18380,7 +18382,7 @@
         <v>497700</v>
       </c>
     </row>
-    <row r="467" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A467">
         <v>7.0609999999999999</v>
       </c>
@@ -18394,7 +18396,7 @@
         <v>525000</v>
       </c>
     </row>
-    <row r="468" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A468">
         <v>5.7619999999999996</v>
       </c>
@@ -18408,7 +18410,7 @@
         <v>457800</v>
       </c>
     </row>
-    <row r="469" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A469">
         <v>5.8710000000000004</v>
       </c>
@@ -18422,7 +18424,7 @@
         <v>432600</v>
       </c>
     </row>
-    <row r="470" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A470">
         <v>6.3120000000000003</v>
       </c>
@@ -18436,7 +18438,7 @@
         <v>445200</v>
       </c>
     </row>
-    <row r="471" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A471">
         <v>6.1139999999999999</v>
       </c>
@@ -18450,7 +18452,7 @@
         <v>401100</v>
       </c>
     </row>
-    <row r="472" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A472">
         <v>5.9050000000000002</v>
       </c>
@@ -18464,7 +18466,7 @@
         <v>432600</v>
       </c>
     </row>
-    <row r="473" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A473">
         <v>5.4539999999999997</v>
       </c>
@@ -18478,7 +18480,7 @@
         <v>319200</v>
       </c>
     </row>
-    <row r="474" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A474">
         <v>5.4139999999999997</v>
       </c>
@@ -18492,7 +18494,7 @@
         <v>147000</v>
       </c>
     </row>
-    <row r="475" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A475">
         <v>5.093</v>
       </c>
@@ -18506,7 +18508,7 @@
         <v>170100</v>
       </c>
     </row>
-    <row r="476" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A476">
         <v>5.9829999999999997</v>
       </c>
@@ -18520,7 +18522,7 @@
         <v>285600</v>
       </c>
     </row>
-    <row r="477" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A477">
         <v>5.9829999999999997</v>
       </c>
@@ -18534,7 +18536,7 @@
         <v>422100</v>
       </c>
     </row>
-    <row r="478" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A478">
         <v>5.7069999999999999</v>
       </c>
@@ -18548,7 +18550,7 @@
         <v>457800</v>
       </c>
     </row>
-    <row r="479" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A479">
         <v>5.9260000000000002</v>
       </c>
@@ -18562,7 +18564,7 @@
         <v>514500</v>
       </c>
     </row>
-    <row r="480" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A480">
         <v>5.67</v>
       </c>
@@ -18576,7 +18578,7 @@
         <v>485100</v>
       </c>
     </row>
-    <row r="481" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A481">
         <v>5.39</v>
       </c>
@@ -18590,7 +18592,7 @@
         <v>413700</v>
       </c>
     </row>
-    <row r="482" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A482">
         <v>5.7939999999999996</v>
       </c>
@@ -18604,7 +18606,7 @@
         <v>384300</v>
       </c>
     </row>
-    <row r="483" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A483">
         <v>6.0190000000000001</v>
       </c>
@@ -18618,7 +18620,7 @@
         <v>445200</v>
       </c>
     </row>
-    <row r="484" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A484">
         <v>5.569</v>
       </c>
@@ -18632,7 +18634,7 @@
         <v>367500</v>
       </c>
     </row>
-    <row r="485" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A485">
         <v>6.0270000000000001</v>
       </c>
@@ -18646,7 +18648,7 @@
         <v>352800</v>
       </c>
     </row>
-    <row r="486" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A486">
         <v>6.593</v>
       </c>
@@ -18660,7 +18662,7 @@
         <v>470400</v>
       </c>
     </row>
-    <row r="487" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A487">
         <v>6.12</v>
       </c>
@@ -18674,7 +18676,7 @@
         <v>432600</v>
       </c>
     </row>
-    <row r="488" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A488">
         <v>6.976</v>
       </c>
@@ -18688,7 +18690,7 @@
         <v>501900</v>
       </c>
     </row>
-    <row r="489" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A489">
         <v>6.7939999999999996</v>
       </c>
@@ -18702,7 +18704,7 @@
         <v>462000</v>
       </c>
     </row>
-    <row r="490" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A490">
         <v>6.03</v>
       </c>
@@ -18717,6 +18719,19 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="C1:C490">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="14.7"/>
+        <filter val="14.8"/>
+        <filter val="14.9"/>
+        <filter val="15.1"/>
+        <filter val="15.2"/>
+        <filter val="15.3"/>
+        <filter val="15.5"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>